<commit_message>
Added functionality to create survey_manifest and also allow for dynamic response creation from csv or database
</commit_message>
<xml_diff>
--- a/Excel/prismcss.xlsx
+++ b/Excel/prismcss.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GeoffOffline\GiSTConfigX\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DD7A27-6115-4C47-AACE-21807276509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC0FFD9-1CA6-4DAF-BB8B-A29168F8A8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="891" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="891" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hh_info_dd" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="155">
   <si>
     <t>Skip</t>
   </si>
@@ -228,23 +228,6 @@
   </si>
   <si>
     <t>Responses</t>
-  </si>
-  <si>
-    <t>1:Busoga
-2:Bukedi
-3:Bugisu
-4:Teso
-5:Karamoja
-6:Lango
-7:Acholi
-8:West Nile
-9:Bunyoro
-10:Tooro
-11:Kigezi
-12:Ankole
-13:South Buganda
-14:North Buganda
-15:Kampala</t>
   </si>
   <si>
     <t>Datetime stamp:automatically generated</t>
@@ -604,6 +587,49 @@
   ],
   "incrementLength": 0
 }</t>
+  </si>
+  <si>
+    <t>source: csv
+file: mrcvillage.csv
+filter: region = [[region]]
+display: mrcname
+value: mrccode</t>
+  </si>
+  <si>
+    <t>source: database
+table: sleeping_structure
+filter: hhid = [[hhid]]
+display: structurelabel
+value: structurenum</t>
+  </si>
+  <si>
+    <t>source: database
+table: hh_members
+filter: hhid = [[hhid]]
+display: participantsname
+value: linenum</t>
+  </si>
+  <si>
+    <t>source: csv
+file: mrcvillage.csv
+filter: region = [[region]]
+filter: mrccode = [[mrccode]]
+display: villagename
+value: vcode</t>
+  </si>
+  <si>
+    <t>1:Busoga
+2:Bukedi
+4:Teso
+5:Karamoja
+6:Lango
+7:Acholi
+8:West Nile
+9:Bunyoro
+10:Tooro
+11:Kigezi
+14:North Buganda
+15:Kampala</t>
   </si>
 </sst>
 </file>
@@ -782,7 +808,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -931,11 +957,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1287,9 +1309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1331,22 +1353,22 @@
         <v>60</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="M1" s="14" t="s">
         <v>0</v>
@@ -1356,32 +1378,32 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
+      <c r="A2" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
     </row>
     <row r="3" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>20</v>
@@ -1396,10 +1418,10 @@
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
       <c r="N3" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="15" customFormat="1" ht="216" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="15" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>47</v>
       </c>
@@ -1407,14 +1429,14 @@
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -1425,7 +1447,7 @@
       <c r="M4" s="22"/>
       <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>42</v>
       </c>
@@ -1433,13 +1455,15 @@
         <v>5</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>150</v>
+      </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
@@ -1448,10 +1472,10 @@
       <c r="L5" s="21"/>
       <c r="M5" s="22"/>
       <c r="N5" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>43</v>
       </c>
@@ -1459,13 +1483,15 @@
         <v>5</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -1474,7 +1500,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
       <c r="N6" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -1482,10 +1508,10 @@
         <v>39</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>40</v>
@@ -1514,13 +1540,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -1532,18 +1558,18 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>11</v>
@@ -1559,7 +1585,7 @@
         <v>399999999</v>
       </c>
       <c r="I9" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
@@ -1575,14 +1601,14 @@
         <v>5</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -1592,7 +1618,7 @@
       <c r="L10" s="25"/>
       <c r="M10" s="17"/>
       <c r="N10" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="27" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -1603,14 +1629,14 @@
         <v>5</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -1619,29 +1645,29 @@
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
       <c r="M11" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N11" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
+      <c r="A12" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
     </row>
     <row r="13" spans="1:14" s="15" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
@@ -1651,14 +1677,14 @@
         <v>5</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -1673,13 +1699,13 @@
     </row>
     <row r="14" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>49</v>
@@ -1703,13 +1729,13 @@
     </row>
     <row r="15" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>35</v>
@@ -1730,7 +1756,7 @@
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
       <c r="N15" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1738,10 +1764,10 @@
         <v>36</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>37</v>
@@ -1762,21 +1788,21 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="15" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>104</v>
-      </c>
       <c r="D17" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
@@ -1790,22 +1816,22 @@
       <c r="N17" s="40"/>
     </row>
     <row r="18" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
+      <c r="A18" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
     </row>
     <row r="19" spans="1:14" s="35" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="25" t="s">
@@ -1815,14 +1841,14 @@
         <v>5</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>31</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -1834,35 +1860,35 @@
       <c r="N19" s="17"/>
     </row>
     <row r="20" spans="1:14" s="15" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
+      <c r="A20" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
     </row>
     <row r="21" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>116</v>
       </c>
       <c r="E21" s="29">
         <v>80</v>
@@ -1879,16 +1905,16 @@
     </row>
     <row r="22" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
@@ -1903,16 +1929,16 @@
     </row>
     <row r="23" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" s="45"/>
       <c r="F23" s="45"/>
@@ -1927,16 +1953,16 @@
     </row>
     <row r="24" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="45" t="s">
         <v>118</v>
-      </c>
-      <c r="B24" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>119</v>
       </c>
       <c r="E24" s="45"/>
       <c r="F24" s="45"/>
@@ -1951,16 +1977,16 @@
     </row>
     <row r="25" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>120</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="45" t="s">
-        <v>121</v>
       </c>
       <c r="E25" s="45"/>
       <c r="F25" s="45"/>
@@ -1978,13 +2004,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="49" t="s">
-        <v>68</v>
-      </c>
       <c r="D26" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
@@ -2063,22 +2089,22 @@
         <v>60</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>0</v>
@@ -2092,10 +2118,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>20</v>
@@ -2110,7 +2136,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2118,10 +2144,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -2142,13 +2168,13 @@
         <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2166,13 +2192,13 @@
         <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="2">
         <v>80</v>
@@ -2195,14 +2221,14 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2221,14 +2247,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2240,35 +2266,35 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
+      <c r="A8" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>116</v>
       </c>
       <c r="E9" s="29">
         <v>80</v>
@@ -2285,16 +2311,16 @@
     </row>
     <row r="10" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
@@ -2309,16 +2335,16 @@
     </row>
     <row r="11" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
@@ -2333,16 +2359,16 @@
     </row>
     <row r="12" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>118</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>119</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
@@ -2357,16 +2383,16 @@
     </row>
     <row r="13" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>120</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>121</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
@@ -2384,13 +2410,13 @@
         <v>8</v>
       </c>
       <c r="B14" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>68</v>
-      </c>
       <c r="D14" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
@@ -2421,7 +2447,7 @@
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2431,8 +2457,7 @@
     <col min="3" max="3" width="13.21875" style="38" customWidth="1"/>
     <col min="4" max="4" width="52.44140625" style="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="57" style="38" customWidth="1"/>
     <col min="8" max="8" width="11.77734375" style="38" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" style="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.21875" style="38" bestFit="1" customWidth="1"/>
@@ -2463,22 +2488,22 @@
         <v>60</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="M1" s="14" t="s">
         <v>0</v>
@@ -2492,10 +2517,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>20</v>
@@ -2510,7 +2535,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2518,10 +2543,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>11</v>
@@ -2542,13 +2567,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" s="36"/>
       <c r="F4" s="17"/>
@@ -2560,7 +2585,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2568,10 +2593,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>45</v>
@@ -2597,14 +2622,14 @@
         <v>5</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>46</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -2620,13 +2645,13 @@
         <v>26</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>70</v>
-      </c>
       <c r="D7" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" s="17">
         <v>3</v>
@@ -2645,7 +2670,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="1:14" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" s="15" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
@@ -2653,13 +2678,15 @@
         <v>5</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="23"/>
+      <c r="F8" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
@@ -2668,39 +2695,39 @@
       <c r="L8" s="23"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
+      <c r="A9" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
     </row>
     <row r="10" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>116</v>
       </c>
       <c r="E10" s="29">
         <v>80</v>
@@ -2717,16 +2744,16 @@
     </row>
     <row r="11" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="45"/>
       <c r="F11" s="45"/>
@@ -2741,16 +2768,16 @@
     </row>
     <row r="12" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="45"/>
@@ -2765,16 +2792,16 @@
     </row>
     <row r="13" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>118</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>119</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
@@ -2789,16 +2816,16 @@
     </row>
     <row r="14" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="45" t="s">
         <v>120</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>121</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
@@ -2816,13 +2843,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="49" t="s">
-        <v>68</v>
-      </c>
       <c r="D15" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
@@ -2854,7 +2881,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2895,22 +2922,22 @@
         <v>60</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>80</v>
       </c>
       <c r="M1" s="39" t="s">
         <v>0</v>
@@ -2924,10 +2951,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>20</v>
@@ -2942,7 +2969,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2950,10 +2977,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>11</v>
@@ -2976,10 +3003,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>28</v>
@@ -3005,14 +3032,14 @@
         <v>5</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
@@ -3032,10 +3059,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>3</v>
@@ -3051,27 +3078,27 @@
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="56"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="54"/>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
@@ -3081,14 +3108,14 @@
         <v>5</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -3108,16 +3135,18 @@
         <v>32</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="23"/>
+      <c r="F9" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
@@ -3128,10 +3157,10 @@
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>54</v>
       </c>
@@ -3139,13 +3168,15 @@
         <v>5</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -3156,35 +3187,35 @@
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
+      <c r="A11" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
     </row>
     <row r="12" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>116</v>
       </c>
       <c r="E12" s="29">
         <v>80</v>
@@ -3201,16 +3232,16 @@
     </row>
     <row r="13" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
@@ -3225,16 +3256,16 @@
     </row>
     <row r="14" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
@@ -3249,16 +3280,16 @@
     </row>
     <row r="15" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>118</v>
-      </c>
-      <c r="B15" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>119</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
@@ -3273,16 +3304,16 @@
     </row>
     <row r="16" spans="1:14" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="45" t="s">
         <v>120</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>121</v>
       </c>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
@@ -3300,13 +3331,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="49" t="s">
-        <v>68</v>
-      </c>
       <c r="D17" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" s="45"/>
       <c r="F17" s="45"/>
@@ -3335,22 +3366,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633949F3-52B4-46B1-9019-8AEA66858D1D}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
@@ -3359,208 +3390,208 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C1" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="E1" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="J1" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="M1" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="N1" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="50" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="26">
+        <v>10</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="27">
+      <c r="D2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="E2" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26">
+        <v>0</v>
+      </c>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26">
+        <v>0</v>
+      </c>
+      <c r="M2" s="26">
+        <v>0</v>
+      </c>
+      <c r="N2" s="26"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="26">
+        <v>20</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C3" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26">
+        <v>0</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="H3" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="26">
+        <v>1</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="26">
+        <v>1</v>
+      </c>
+      <c r="M3" s="26">
+        <v>2</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="26">
+        <v>30</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="27">
+      <c r="C4" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26">
+        <v>0</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="26">
         <v>1</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="K4" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4" s="26">
+        <v>1</v>
+      </c>
+      <c r="M4" s="26">
+        <v>2</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="26">
+        <v>40</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26">
+        <v>0</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27">
-        <v>0</v>
-      </c>
-      <c r="J2" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27">
-        <v>0</v>
-      </c>
-      <c r="M2" s="27">
-        <v>0</v>
-      </c>
-      <c r="N2" s="27"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
-        <v>20</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="27">
-        <v>0</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="27">
+      <c r="H5" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="26">
         <v>1</v>
       </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="L3" s="27">
+      <c r="K5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="26">
         <v>1</v>
       </c>
-      <c r="M3" s="27">
+      <c r="M5" s="26">
         <v>2</v>
       </c>
-      <c r="N3" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
-        <v>30</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="27">
-        <v>0</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="27">
-        <v>1</v>
-      </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="L4" s="27">
-        <v>1</v>
-      </c>
-      <c r="M4" s="27">
-        <v>2</v>
-      </c>
-      <c r="N4" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
-        <v>40</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="N5" s="26" t="s">
         <v>147</v>
-      </c>
-      <c r="E5" s="27">
-        <v>0</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="27">
-        <v>1</v>
-      </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="27">
-        <v>1</v>
-      </c>
-      <c r="M5" s="27">
-        <v>2</v>
-      </c>
-      <c r="N5" s="27" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>